<commit_message>
Changed excel file for Watchlist
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Watchlist.xlsx
+++ b/src/test/resources/xls/Watchlist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -552,9 +552,6 @@
   </si>
   <si>
     <t>Verify that document count gets decreased in the watchlist page when an item is deleted from watchlist</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Watchlist030</t>
@@ -981,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1022,7 +1019,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>30</v>
@@ -1039,7 +1036,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>30</v>
@@ -1056,7 +1053,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
@@ -1073,7 +1070,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>30</v>
@@ -1090,7 +1087,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>30</v>
@@ -1107,7 +1104,7 @@
         <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>30</v>
@@ -1124,7 +1121,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>30</v>
@@ -1141,7 +1138,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>30</v>
@@ -1158,7 +1155,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>30</v>
@@ -1175,7 +1172,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>30</v>
@@ -1192,7 +1189,7 @@
         <v>92</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>30</v>
@@ -1209,7 +1206,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>30</v>
@@ -1226,7 +1223,7 @@
         <v>93</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>30</v>
@@ -1243,7 +1240,7 @@
         <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>30</v>
@@ -1260,7 +1257,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>30</v>
@@ -1277,7 +1274,7 @@
         <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>30</v>
@@ -1294,7 +1291,7 @@
         <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>30</v>
@@ -1311,7 +1308,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>30</v>
@@ -1328,7 +1325,7 @@
         <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>30</v>
@@ -1345,7 +1342,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>30</v>
@@ -1362,7 +1359,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>30</v>
@@ -1379,7 +1376,7 @@
         <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>30</v>
@@ -1396,7 +1393,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>30</v>
@@ -1413,7 +1410,7 @@
         <v>56</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>30</v>
@@ -1430,7 +1427,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>30</v>
@@ -1447,7 +1444,7 @@
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>30</v>
@@ -1464,7 +1461,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>30</v>
@@ -1481,7 +1478,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>30</v>
@@ -1498,7 +1495,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>30</v>
@@ -1506,43 +1503,43 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>91</v>
@@ -1551,13 +1548,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Test case updated in watchlist.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Watchlist.xlsx
+++ b/src/test/resources/xls/Watchlist.xlsx
@@ -88,10 +88,6 @@
 ||OPQA-621</t>
   </si>
   <si>
-    <t>OPQA-329
-||OPQA-621</t>
-  </si>
-  <si>
     <t>OPQA-1108</t>
   </si>
   <si>
@@ -588,6 +584,10 @@
   </si>
   <si>
     <t>Verify that deep linking is working correctly for particular watchlist page when user logs in using Social(FB or LI) account</t>
+  </si>
+  <si>
+    <t>OPQA-329
+||OPQA-622</t>
   </si>
 </sst>
 </file>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1010,160 +1010,160 @@
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45">
       <c r="A5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
       <c r="A8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45">
       <c r="A9" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -1172,32 +1172,32 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45">
       <c r="A12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
       <c r="A13" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1206,134 +1206,134 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
       <c r="A15" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45">
       <c r="A16" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45">
       <c r="A17" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45">
       <c r="A18" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30">
       <c r="A19" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45">
       <c r="A20" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
@@ -1342,15 +1342,15 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
@@ -1359,32 +1359,32 @@
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
@@ -1393,171 +1393,171 @@
         <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30">
       <c r="A28" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30">
       <c r="A29" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30">
       <c r="A30" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D34" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E34" s="1"/>
     </row>

</xml_diff>

<commit_message>
changes for watchlist034 script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Watchlist.xlsx
+++ b/src/test/resources/xls/Watchlist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -588,6 +588,15 @@
   <si>
     <t>OPQA-329
 ||OPQA-622</t>
+  </si>
+  <si>
+    <t>OPQA-322</t>
+  </si>
+  <si>
+    <t>Verify that user is able to comment on his watchlist items</t>
+  </si>
+  <si>
+    <t>Watchlist034</t>
   </si>
 </sst>
 </file>
@@ -976,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1560,6 +1569,21 @@
         <v>90</v>
       </c>
       <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New watchlist script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Watchlist.xlsx
+++ b/src/test/resources/xls/Watchlist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="112">
   <si>
     <t>TCID</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>Watchlist034</t>
+  </si>
+  <si>
+    <t>OPQA-620</t>
+  </si>
+  <si>
+    <t>Verify that user is able to comment on an item contained in public watchlist of some other user</t>
+  </si>
+  <si>
+    <t>Watchlist035</t>
   </si>
 </sst>
 </file>
@@ -985,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1584,6 +1593,21 @@
         <v>90</v>
       </c>
       <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>